<commit_message>
created new product classes
</commit_message>
<xml_diff>
--- a/Products.xlsx
+++ b/Products.xlsx
@@ -149,9 +149,6 @@
     <t>Double magazine holder for ???</t>
   </si>
   <si>
-    <t>Sam Brown Belt</t>
-  </si>
-  <si>
     <t>200-1</t>
   </si>
   <si>
@@ -186,6 +183,9 @@
   </si>
   <si>
     <t>SKU</t>
+  </si>
+  <si>
+    <t>Sam Browne Belt</t>
   </si>
 </sst>
 </file>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,10 +588,10 @@
         <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -642,10 +642,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -653,21 +653,21 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>44</v>
-      </c>
-      <c r="D8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>14</v>
@@ -676,12 +676,12 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>15</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
@@ -774,13 +774,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
         <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -788,13 +788,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
         <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -802,13 +802,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>